<commit_message>
Exclui canvas e backlog antigos e atualizei apresentação
</commit_message>
<xml_diff>
--- a/Sprint 1/Canvas , Backlog & User Stories/PBC - Product Backlog Classified V2.xlsx
+++ b/Sprint 1/Canvas , Backlog & User Stories/PBC - Product Backlog Classified V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renna\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/bruna_martins_b_melo_accenture_com/Documents/Documents/Prepta/Prepta/Sprint 1/Canvas , Backlog &amp; User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABCEF65-3199-4558-9F76-1C4BCDB7EC6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{FABCEF65-3199-4558-9F76-1C4BCDB7EC6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{6E3B1629-92CD-453E-AA2E-CAA626D2ECE7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PBC" sheetId="15" r:id="rId1"/>
@@ -577,7 +577,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -736,6 +736,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Exu"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -829,7 +834,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -922,6 +927,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -947,7 +978,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1133,13 +1164,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="14" borderId="4" xfId="21" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1163,29 +1187,43 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="22">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hiperlink" xfId="21" builtinId="8"/>
-    <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hiperlink Visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="55">
@@ -2337,36 +2375,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:K51"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="23.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="23.15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="3.90625" style="14" customWidth="1"/>
     <col min="2" max="2" width="11" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.6640625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="78.88671875" style="14" customWidth="1"/>
-    <col min="5" max="5" width="0.6640625" style="16" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" style="14" customWidth="1"/>
-    <col min="9" max="10" width="8.88671875" style="14"/>
-    <col min="11" max="11" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="14"/>
+    <col min="3" max="3" width="42.6328125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="78.90625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="0.6328125" style="16" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="15.453125" style="14" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.36328125" style="14" customWidth="1"/>
+    <col min="9" max="10" width="8.90625" style="14"/>
+    <col min="11" max="11" width="13.6328125" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.90625" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="19.5" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:11" ht="89.25" customHeight="1" thickBot="1">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="69"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="67"/>
     </row>
     <row r="3" spans="2:11" ht="9.9" customHeight="1" thickBot="1"/>
     <row r="4" spans="2:11" s="23" customFormat="1" ht="24.9" customHeight="1" thickBot="1">
@@ -2392,7 +2430,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:11" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="5" spans="2:11" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B5" s="24" t="s">
         <v>43</v>
       </c>
@@ -2409,7 +2447,7 @@
       <c r="G5" s="27"/>
       <c r="H5" s="27"/>
     </row>
-    <row r="6" spans="2:11" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="6" spans="2:11" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B6" s="24" t="s">
         <v>43</v>
       </c>
@@ -2428,7 +2466,7 @@
       </c>
       <c r="H6" s="27"/>
     </row>
-    <row r="7" spans="2:11" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="7" spans="2:11" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B7" s="24" t="s">
         <v>43</v>
       </c>
@@ -2445,7 +2483,7 @@
       </c>
       <c r="H7" s="27"/>
     </row>
-    <row r="8" spans="2:11" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="8" spans="2:11" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B8" s="24" t="s">
         <v>43</v>
       </c>
@@ -2482,7 +2520,7 @@
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
     </row>
-    <row r="10" spans="2:11" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="10" spans="2:11" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B10" s="24" t="s">
         <v>43</v>
       </c>
@@ -2499,7 +2537,7 @@
       <c r="G10" s="27"/>
       <c r="H10" s="27"/>
     </row>
-    <row r="11" spans="2:11" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="11" spans="2:11" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B11" s="24" t="s">
         <v>43</v>
       </c>
@@ -2516,7 +2554,7 @@
       </c>
       <c r="H11" s="27"/>
     </row>
-    <row r="12" spans="2:11" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="12" spans="2:11" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B12" s="24" t="s">
         <v>43</v>
       </c>
@@ -2533,7 +2571,7 @@
       </c>
       <c r="H12" s="27"/>
     </row>
-    <row r="13" spans="2:11" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="13" spans="2:11" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B13" s="24" t="s">
         <v>43</v>
       </c>
@@ -2550,7 +2588,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="2:11" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="14" spans="2:11" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B14" s="24" t="s">
         <v>43</v>
       </c>
@@ -2567,7 +2605,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:11" s="28" customFormat="1" ht="29.4" thickBot="1">
+    <row r="15" spans="2:11" s="28" customFormat="1" ht="29.5" thickBot="1">
       <c r="B15" s="24" t="s">
         <v>43</v>
       </c>
@@ -2582,7 +2620,7 @@
       <c r="G15" s="33"/>
       <c r="H15" s="27"/>
     </row>
-    <row r="16" spans="2:11" s="28" customFormat="1" ht="29.4" thickBot="1">
+    <row r="16" spans="2:11" s="28" customFormat="1" ht="29.5" thickBot="1">
       <c r="B16" s="24" t="s">
         <v>43</v>
       </c>
@@ -2599,7 +2637,7 @@
       </c>
       <c r="H16" s="27"/>
     </row>
-    <row r="17" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="17" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B17" s="24" t="s">
         <v>43</v>
       </c>
@@ -2612,7 +2650,7 @@
       <c r="G17" s="27"/>
       <c r="H17" s="27"/>
     </row>
-    <row r="18" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="18" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B18" s="24" t="s">
         <v>43</v>
       </c>
@@ -2625,7 +2663,7 @@
       <c r="G18" s="27"/>
       <c r="H18" s="27"/>
     </row>
-    <row r="19" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="19" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B19" s="24" t="s">
         <v>43</v>
       </c>
@@ -2638,7 +2676,7 @@
       <c r="G19" s="27"/>
       <c r="H19" s="27"/>
     </row>
-    <row r="20" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="20" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B20" s="24" t="s">
         <v>43</v>
       </c>
@@ -2651,7 +2689,7 @@
       <c r="G20" s="27"/>
       <c r="H20" s="27"/>
     </row>
-    <row r="21" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="21" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B21" s="24" t="s">
         <v>43</v>
       </c>
@@ -2664,7 +2702,7 @@
       <c r="G21" s="27"/>
       <c r="H21" s="27"/>
     </row>
-    <row r="22" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="22" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B22" s="24" t="s">
         <v>43</v>
       </c>
@@ -2677,7 +2715,7 @@
       <c r="G22" s="27"/>
       <c r="H22" s="27"/>
     </row>
-    <row r="23" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="23" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B23" s="24" t="s">
         <v>43</v>
       </c>
@@ -2690,7 +2728,7 @@
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
     </row>
-    <row r="24" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="24" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B24" s="24" t="s">
         <v>43</v>
       </c>
@@ -2703,7 +2741,7 @@
       <c r="G24" s="27"/>
       <c r="H24" s="27"/>
     </row>
-    <row r="25" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="25" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B25" s="24" t="s">
         <v>43</v>
       </c>
@@ -2714,7 +2752,7 @@
       <c r="G25" s="27"/>
       <c r="H25" s="27"/>
     </row>
-    <row r="26" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="26" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B26" s="24" t="s">
         <v>43</v>
       </c>
@@ -2725,7 +2763,7 @@
       <c r="G26" s="27"/>
       <c r="H26" s="27"/>
     </row>
-    <row r="27" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="27" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B27" s="24" t="s">
         <v>43</v>
       </c>
@@ -2736,7 +2774,7 @@
       <c r="G27" s="27"/>
       <c r="H27" s="27"/>
     </row>
-    <row r="28" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="28" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B28" s="24" t="s">
         <v>43</v>
       </c>
@@ -2747,7 +2785,7 @@
       <c r="G28" s="27"/>
       <c r="H28" s="27"/>
     </row>
-    <row r="29" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="29" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B29" s="24" t="s">
         <v>43</v>
       </c>
@@ -2758,7 +2796,7 @@
       <c r="G29" s="27"/>
       <c r="H29" s="27"/>
     </row>
-    <row r="30" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="30" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B30" s="24" t="s">
         <v>43</v>
       </c>
@@ -2769,7 +2807,7 @@
       <c r="G30" s="27"/>
       <c r="H30" s="27"/>
     </row>
-    <row r="31" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="31" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B31" s="24" t="s">
         <v>43</v>
       </c>
@@ -2780,7 +2818,7 @@
       <c r="G31" s="27"/>
       <c r="H31" s="27"/>
     </row>
-    <row r="32" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="32" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B32" s="24" t="s">
         <v>43</v>
       </c>
@@ -2791,7 +2829,7 @@
       <c r="G32" s="27"/>
       <c r="H32" s="27"/>
     </row>
-    <row r="33" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="33" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B33" s="24" t="s">
         <v>43</v>
       </c>
@@ -2802,7 +2840,7 @@
       <c r="G33" s="27"/>
       <c r="H33" s="27"/>
     </row>
-    <row r="34" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1" thickBot="1">
+    <row r="34" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1" thickBot="1">
       <c r="B34" s="24" t="s">
         <v>43</v>
       </c>
@@ -2813,87 +2851,87 @@
       <c r="G34" s="27"/>
       <c r="H34" s="27"/>
     </row>
-    <row r="35" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="35" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C35" s="35"/>
       <c r="E35" s="36"/>
       <c r="G35" s="37"/>
     </row>
-    <row r="36" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="36" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C36" s="35"/>
       <c r="E36" s="36"/>
       <c r="G36" s="37"/>
     </row>
-    <row r="37" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="37" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C37" s="35"/>
       <c r="E37" s="36"/>
       <c r="G37" s="37"/>
     </row>
-    <row r="38" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="38" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C38" s="35"/>
       <c r="E38" s="36"/>
       <c r="G38" s="37"/>
     </row>
-    <row r="39" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="39" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C39" s="35"/>
       <c r="E39" s="36"/>
       <c r="G39" s="37"/>
     </row>
-    <row r="40" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="40" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C40" s="35"/>
       <c r="E40" s="36"/>
       <c r="G40" s="37"/>
     </row>
-    <row r="41" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="41" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C41" s="35"/>
       <c r="E41" s="36"/>
       <c r="G41" s="37"/>
     </row>
-    <row r="42" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="42" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C42" s="35"/>
       <c r="E42" s="36"/>
       <c r="G42" s="37"/>
     </row>
-    <row r="43" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="43" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C43" s="35"/>
       <c r="E43" s="36"/>
       <c r="G43" s="37"/>
     </row>
-    <row r="44" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="44" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C44" s="35"/>
       <c r="E44" s="36"/>
       <c r="G44" s="37"/>
     </row>
-    <row r="45" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="45" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C45" s="35"/>
       <c r="E45" s="36"/>
       <c r="G45" s="37"/>
     </row>
-    <row r="46" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="46" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C46" s="35"/>
       <c r="E46" s="36"/>
       <c r="G46" s="37"/>
     </row>
-    <row r="47" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="47" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C47" s="35"/>
       <c r="E47" s="36"/>
       <c r="G47" s="37"/>
     </row>
-    <row r="48" spans="2:8" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="48" spans="2:8" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C48" s="35"/>
       <c r="E48" s="36"/>
       <c r="G48" s="37"/>
     </row>
-    <row r="49" spans="3:7" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="49" spans="3:7" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C49" s="35"/>
       <c r="E49" s="36"/>
       <c r="G49" s="37"/>
     </row>
-    <row r="50" spans="3:7" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="50" spans="3:7" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C50" s="35"/>
       <c r="E50" s="36"/>
       <c r="G50" s="37"/>
     </row>
-    <row r="51" spans="3:7" s="28" customFormat="1" ht="23.1" customHeight="1">
+    <row r="51" spans="3:7" s="28" customFormat="1" ht="23.15" customHeight="1">
       <c r="C51" s="35"/>
       <c r="E51" s="36"/>
       <c r="G51" s="37"/>
@@ -3012,12 +3050,12 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="52.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.88671875" style="2"/>
+    <col min="1" max="1" width="52.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.90625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="3" customFormat="1" ht="30" customHeight="1">
@@ -3122,7 +3160,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="23.4">
+    <row r="17" spans="1:2" ht="23.5">
       <c r="A17" s="11" t="s">
         <v>47</v>
       </c>
@@ -3130,7 +3168,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="23.4">
+    <row r="18" spans="1:2" ht="23.5">
       <c r="A18" s="11" t="s">
         <v>48</v>
       </c>
@@ -3138,7 +3176,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="23.4">
+    <row r="19" spans="1:2" ht="23.5">
       <c r="A19" s="11" t="s">
         <v>49</v>
       </c>
@@ -3146,7 +3184,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="23.4">
+    <row r="20" spans="1:2" ht="23.5">
       <c r="A20" s="11" t="s">
         <v>50</v>
       </c>
@@ -3154,7 +3192,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="23.4">
+    <row r="21" spans="1:2" ht="23.5">
       <c r="A21" s="11" t="s">
         <v>51</v>
       </c>
@@ -3162,7 +3200,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="23.4">
+    <row r="22" spans="1:2" ht="23.5">
       <c r="A22" s="11" t="s">
         <v>52</v>
       </c>
@@ -3170,7 +3208,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="23.4">
+    <row r="23" spans="1:2" ht="23.5">
       <c r="A23" s="11" t="s">
         <v>53</v>
       </c>
@@ -3178,7 +3216,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="23.4">
+    <row r="24" spans="1:2" ht="23.5">
       <c r="A24" s="11" t="s">
         <v>54</v>
       </c>
@@ -3186,7 +3224,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="23.4">
+    <row r="25" spans="1:2" ht="23.5">
       <c r="A25" s="11" t="s">
         <v>55</v>
       </c>
@@ -3194,7 +3232,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="23.4">
+    <row r="26" spans="1:2" ht="23.5">
       <c r="A26" s="11" t="s">
         <v>65</v>
       </c>
@@ -3202,7 +3240,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="23.4">
+    <row r="27" spans="1:2" ht="23.5">
       <c r="A27" s="11" t="s">
         <v>73</v>
       </c>
@@ -3221,24 +3259,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94976FE-4B40-493B-8530-5823F3478496}">
   <dimension ref="C2:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="G10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.77734375" customWidth="1"/>
-    <col min="5" max="5" width="54.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.54296875" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" customWidth="1"/>
+    <col min="5" max="5" width="54.90625" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" customWidth="1"/>
+    <col min="7" max="7" width="16.08984375" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" customWidth="1"/>
     <col min="10" max="10" width="38" customWidth="1"/>
-    <col min="11" max="11" width="37.88671875" customWidth="1"/>
-    <col min="12" max="12" width="52.6640625" customWidth="1"/>
-    <col min="13" max="13" width="16.5546875" customWidth="1"/>
-    <col min="14" max="14" width="15.109375" customWidth="1"/>
-    <col min="15" max="16" width="14.21875" customWidth="1"/>
+    <col min="11" max="11" width="37.90625" customWidth="1"/>
+    <col min="12" max="12" width="52.6328125" customWidth="1"/>
+    <col min="13" max="13" width="16.54296875" customWidth="1"/>
+    <col min="14" max="14" width="15.08984375" customWidth="1"/>
+    <col min="15" max="16" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:15">
@@ -3469,19 +3507,21 @@
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
-      <c r="H10" s="51" t="s">
+      <c r="H10" s="71" t="s">
         <v>39</v>
       </c>
       <c r="M10" s="60"/>
     </row>
-    <row r="11" spans="3:15" ht="16.2">
-      <c r="J11" s="61" t="s">
+    <row r="11" spans="3:15" ht="18">
+      <c r="H11" s="72"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="K11" s="63" t="s">
+      <c r="K11" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="L11" s="65" t="s">
+      <c r="L11" s="63" t="s">
         <v>15</v>
       </c>
       <c r="M11" s="57" t="s">
@@ -3494,14 +3534,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="3:15" ht="27.6">
-      <c r="J12" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="64" t="s">
+    <row r="12" spans="3:15" ht="28">
+      <c r="H12" s="72"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="62" t="s">
         <v>135</v>
       </c>
-      <c r="L12" s="66" t="s">
+      <c r="L12" s="64" t="s">
         <v>121</v>
       </c>
       <c r="M12" s="59" t="s">
@@ -3510,14 +3552,16 @@
       <c r="N12" s="58"/>
       <c r="O12" s="58"/>
     </row>
-    <row r="13" spans="3:15" ht="24.6">
-      <c r="J13" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K13" s="64" t="s">
+    <row r="13" spans="3:15" ht="25">
+      <c r="H13" s="72"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K13" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="L13" s="66" t="s">
+      <c r="L13" s="64" t="s">
         <v>122</v>
       </c>
       <c r="M13" s="59" t="s">
@@ -3526,14 +3570,16 @@
       <c r="N13" s="58"/>
       <c r="O13" s="58"/>
     </row>
-    <row r="14" spans="3:15" ht="27.6">
-      <c r="J14" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K14" s="64" t="s">
+    <row r="14" spans="3:15" ht="28">
+      <c r="H14" s="72"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="62" t="s">
         <v>137</v>
       </c>
-      <c r="L14" s="66" t="s">
+      <c r="L14" s="64" t="s">
         <v>123</v>
       </c>
       <c r="M14" s="59" t="s">
@@ -3542,14 +3588,16 @@
       <c r="N14" s="58"/>
       <c r="O14" s="58"/>
     </row>
-    <row r="15" spans="3:15" ht="27.6">
-      <c r="J15" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K15" s="64" t="s">
+    <row r="15" spans="3:15" ht="28">
+      <c r="H15" s="72"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="62" t="s">
         <v>139</v>
       </c>
-      <c r="L15" s="66" t="s">
+      <c r="L15" s="64" t="s">
         <v>124</v>
       </c>
       <c r="M15" s="58"/>
@@ -3558,14 +3606,16 @@
       </c>
       <c r="O15" s="58"/>
     </row>
-    <row r="16" spans="3:15" ht="27.6">
-      <c r="J16" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K16" s="64" t="s">
+    <row r="16" spans="3:15" ht="28">
+      <c r="H16" s="72"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="L16" s="66" t="s">
+      <c r="L16" s="64" t="s">
         <v>125</v>
       </c>
       <c r="M16" s="58"/>
@@ -3574,14 +3624,16 @@
       </c>
       <c r="O16" s="58"/>
     </row>
-    <row r="17" spans="10:15" ht="27.6">
-      <c r="J17" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K17" s="64" t="s">
+    <row r="17" spans="8:15" ht="25">
+      <c r="H17" s="72"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="62" t="s">
         <v>141</v>
       </c>
-      <c r="L17" s="66" t="s">
+      <c r="L17" s="64" t="s">
         <v>131</v>
       </c>
       <c r="M17" s="59" t="s">
@@ -3590,14 +3642,16 @@
       <c r="N17" s="58"/>
       <c r="O17" s="58"/>
     </row>
-    <row r="18" spans="10:15" ht="27.6">
-      <c r="J18" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K18" s="64" t="s">
+    <row r="18" spans="8:15" ht="28">
+      <c r="H18" s="72"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" s="62" t="s">
         <v>142</v>
       </c>
-      <c r="L18" s="66" t="s">
+      <c r="L18" s="64" t="s">
         <v>126</v>
       </c>
       <c r="M18" s="58"/>
@@ -3606,14 +3660,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="10:15" ht="41.4">
-      <c r="J19" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K19" s="64" t="s">
+    <row r="19" spans="8:15" ht="28">
+      <c r="H19" s="72"/>
+      <c r="I19" s="68"/>
+      <c r="J19" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="L19" s="66" t="s">
+      <c r="L19" s="64" t="s">
         <v>127</v>
       </c>
       <c r="M19" s="58"/>
@@ -3622,14 +3678,16 @@
       </c>
       <c r="O19" s="58"/>
     </row>
-    <row r="20" spans="10:15" ht="24.6">
-      <c r="J20" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K20" s="64" t="s">
+    <row r="20" spans="8:15" ht="25">
+      <c r="H20" s="72"/>
+      <c r="I20" s="68"/>
+      <c r="J20" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K20" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="L20" s="66" t="s">
+      <c r="L20" s="64" t="s">
         <v>128</v>
       </c>
       <c r="M20" s="58"/>
@@ -3638,14 +3696,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="10:15" ht="41.4">
-      <c r="J21" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K21" s="64" t="s">
+    <row r="21" spans="8:15" ht="28">
+      <c r="H21" s="72"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="L21" s="66" t="s">
+      <c r="L21" s="64" t="s">
         <v>129</v>
       </c>
       <c r="M21" s="58"/>
@@ -3654,14 +3714,16 @@
       </c>
       <c r="O21" s="58"/>
     </row>
-    <row r="22" spans="10:15" ht="27.6">
-      <c r="J22" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K22" s="64" t="s">
+    <row r="22" spans="8:15" ht="25">
+      <c r="H22" s="72"/>
+      <c r="I22" s="68"/>
+      <c r="J22" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K22" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="L22" s="66" t="s">
+      <c r="L22" s="64" t="s">
         <v>130</v>
       </c>
       <c r="M22" s="59" t="s">
@@ -3670,14 +3732,16 @@
       <c r="N22" s="58"/>
       <c r="O22" s="58"/>
     </row>
-    <row r="23" spans="10:15" ht="27.6">
-      <c r="J23" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K23" s="64" t="s">
+    <row r="23" spans="8:15" ht="28">
+      <c r="H23" s="72"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K23" s="62" t="s">
         <v>145</v>
       </c>
-      <c r="L23" s="66" t="s">
+      <c r="L23" s="64" t="s">
         <v>132</v>
       </c>
       <c r="M23" s="59" t="s">
@@ -3686,14 +3750,16 @@
       <c r="N23" s="58"/>
       <c r="O23" s="58"/>
     </row>
-    <row r="24" spans="10:15" ht="27.6">
-      <c r="J24" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="K24" s="64" t="s">
+    <row r="24" spans="8:15" ht="28">
+      <c r="H24" s="72"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="70" t="s">
+        <v>43</v>
+      </c>
+      <c r="K24" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="L24" s="66" t="s">
+      <c r="L24" s="64" t="s">
         <v>134</v>
       </c>
       <c r="M24" s="59"/>

</xml_diff>

<commit_message>
corrigindo alguns erros na apresentação
</commit_message>
<xml_diff>
--- a/Sprint 1/Canvas , Backlog & User Stories/PBC - Product Backlog Classified V2.xlsx
+++ b/Sprint 1/Canvas , Backlog & User Stories/PBC - Product Backlog Classified V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myoffice.accenture.com/personal/bruna_martins_b_melo_accenture_com/Documents/Documents/Prepta/Prepta/Sprint 1/Canvas , Backlog &amp; User Stories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{FABCEF65-3199-4558-9F76-1C4BCDB7EC6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{6E3B1629-92CD-453E-AA2E-CAA626D2ECE7}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{FABCEF65-3199-4558-9F76-1C4BCDB7EC6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{E0A242A8-D896-45F8-BA19-44C3420FB834}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="885" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -498,9 +498,6 @@
     <t>Envio de relatórios sobre desempenho da máquina</t>
   </si>
   <si>
-    <t>O sistema deve notificar o gestor caso algo esteja fora dos padroões</t>
-  </si>
-  <si>
     <t>O sistema deve notificar o atendente caso ele esteja fazendo algo fora do escopo</t>
   </si>
   <si>
@@ -510,18 +507,6 @@
     <t>O site deve ser responsivivo e intuitivo e com cores frias</t>
   </si>
   <si>
-    <t>O sistema devera gerar gráficos para analisar a performance das máquinas utilizadas pelos atendentes</t>
-  </si>
-  <si>
-    <t>O sistema devera notificar o usuário via email</t>
-  </si>
-  <si>
-    <t>O site devera conter uma página de contato com um formulário para o lead fazer perguntas sobre o negócio</t>
-  </si>
-  <si>
-    <t>O site devera ter página de login e cadastro do usuário</t>
-  </si>
-  <si>
     <t>O Sistema deverá captar as informações da máquina</t>
   </si>
   <si>
@@ -568,6 +553,21 @@
   </si>
   <si>
     <t>&lt;Gamification&gt; CC#002</t>
+  </si>
+  <si>
+    <t>O sistema deve notificar o gestor caso algo esteja fora dos padrões</t>
+  </si>
+  <si>
+    <t>O sistema deverá gerar gráficos para analisar a performance das máquinas utilizadas pelos atendentes</t>
+  </si>
+  <si>
+    <t>O sistema deverá notificar o usuário via email</t>
+  </si>
+  <si>
+    <t>O site deverá conter uma página de contato com um formulário para o lead fazer perguntas sobre o negócio</t>
+  </si>
+  <si>
+    <t>O site deverá ter página de login e cadastro do usuário</t>
   </si>
 </sst>
 </file>
@@ -1178,15 +1178,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1201,6 +1192,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2396,15 +2396,15 @@
   <sheetData>
     <row r="1" spans="2:11" ht="19.5" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:11" ht="89.25" customHeight="1" thickBot="1">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="67"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="2:11" ht="9.9" customHeight="1" thickBot="1"/>
     <row r="4" spans="2:11" s="23" customFormat="1" ht="24.9" customHeight="1" thickBot="1">
@@ -3260,7 +3260,7 @@
   <dimension ref="C2:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -3507,19 +3507,19 @@
       </c>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
-      <c r="H10" s="71" t="s">
+      <c r="H10" s="68" t="s">
         <v>39</v>
       </c>
       <c r="M10" s="60"/>
     </row>
     <row r="11" spans="3:15" ht="18">
-      <c r="H11" s="72"/>
-      <c r="I11" s="68"/>
-      <c r="J11" s="69" t="s">
+      <c r="H11" s="69"/>
+      <c r="I11" s="65"/>
+      <c r="J11" s="66" t="s">
         <v>45</v>
       </c>
       <c r="K11" s="61" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L11" s="63" t="s">
         <v>15</v>
@@ -3535,13 +3535,13 @@
       </c>
     </row>
     <row r="12" spans="3:15" ht="28">
-      <c r="H12" s="72"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="70" t="s">
+      <c r="H12" s="69"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K12" s="62" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="L12" s="64" t="s">
         <v>121</v>
@@ -3553,13 +3553,13 @@
       <c r="O12" s="58"/>
     </row>
     <row r="13" spans="3:15" ht="25">
-      <c r="H13" s="72"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="70" t="s">
+      <c r="H13" s="69"/>
+      <c r="I13" s="65"/>
+      <c r="J13" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K13" s="62" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="L13" s="64" t="s">
         <v>122</v>
@@ -3571,16 +3571,16 @@
       <c r="O13" s="58"/>
     </row>
     <row r="14" spans="3:15" ht="28">
-      <c r="H14" s="72"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="70" t="s">
+      <c r="H14" s="69"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K14" s="62" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="L14" s="64" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="M14" s="59" t="s">
         <v>39</v>
@@ -3589,16 +3589,16 @@
       <c r="O14" s="58"/>
     </row>
     <row r="15" spans="3:15" ht="28">
-      <c r="H15" s="72"/>
-      <c r="I15" s="68"/>
-      <c r="J15" s="70" t="s">
+      <c r="H15" s="69"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K15" s="62" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="L15" s="64" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M15" s="58"/>
       <c r="N15" s="59" t="s">
@@ -3607,16 +3607,16 @@
       <c r="O15" s="58"/>
     </row>
     <row r="16" spans="3:15" ht="28">
-      <c r="H16" s="72"/>
-      <c r="I16" s="68"/>
-      <c r="J16" s="70" t="s">
+      <c r="H16" s="69"/>
+      <c r="I16" s="65"/>
+      <c r="J16" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K16" s="62" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="L16" s="64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M16" s="58"/>
       <c r="N16" s="59" t="s">
@@ -3625,16 +3625,16 @@
       <c r="O16" s="58"/>
     </row>
     <row r="17" spans="8:15" ht="25">
-      <c r="H17" s="72"/>
-      <c r="I17" s="68"/>
-      <c r="J17" s="70" t="s">
+      <c r="H17" s="69"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K17" s="62" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="L17" s="64" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="M17" s="59" t="s">
         <v>39</v>
@@ -3643,16 +3643,16 @@
       <c r="O17" s="58"/>
     </row>
     <row r="18" spans="8:15" ht="28">
-      <c r="H18" s="72"/>
-      <c r="I18" s="68"/>
-      <c r="J18" s="70" t="s">
+      <c r="H18" s="69"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K18" s="62" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="L18" s="64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M18" s="58"/>
       <c r="N18" s="58"/>
@@ -3660,17 +3660,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="8:15" ht="28">
-      <c r="H19" s="72"/>
-      <c r="I19" s="68"/>
-      <c r="J19" s="70" t="s">
+    <row r="19" spans="8:15" ht="42">
+      <c r="H19" s="69"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K19" s="62" t="s">
+        <v>138</v>
+      </c>
+      <c r="L19" s="64" t="s">
         <v>143</v>
-      </c>
-      <c r="L19" s="64" t="s">
-        <v>127</v>
       </c>
       <c r="M19" s="58"/>
       <c r="N19" s="59" t="s">
@@ -3679,16 +3679,16 @@
       <c r="O19" s="58"/>
     </row>
     <row r="20" spans="8:15" ht="25">
-      <c r="H20" s="72"/>
-      <c r="I20" s="68"/>
-      <c r="J20" s="70" t="s">
+      <c r="H20" s="69"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K20" s="62" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="L20" s="64" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="M20" s="58"/>
       <c r="N20" s="58"/>
@@ -3696,17 +3696,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="8:15" ht="28">
-      <c r="H21" s="72"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="70" t="s">
+    <row r="21" spans="8:15" ht="42">
+      <c r="H21" s="69"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K21" s="62" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L21" s="64" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="M21" s="58"/>
       <c r="N21" s="59" t="s">
@@ -3715,16 +3715,16 @@
       <c r="O21" s="58"/>
     </row>
     <row r="22" spans="8:15" ht="25">
-      <c r="H22" s="72"/>
-      <c r="I22" s="68"/>
-      <c r="J22" s="70" t="s">
+      <c r="H22" s="69"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K22" s="62" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="L22" s="64" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="M22" s="59" t="s">
         <v>39</v>
@@ -3733,16 +3733,16 @@
       <c r="O22" s="58"/>
     </row>
     <row r="23" spans="8:15" ht="28">
-      <c r="H23" s="72"/>
-      <c r="I23" s="68"/>
-      <c r="J23" s="70" t="s">
+      <c r="H23" s="69"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K23" s="62" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="L23" s="64" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="M23" s="59" t="s">
         <v>39</v>
@@ -3751,16 +3751,16 @@
       <c r="O23" s="58"/>
     </row>
     <row r="24" spans="8:15" ht="28">
-      <c r="H24" s="72"/>
-      <c r="I24" s="68"/>
-      <c r="J24" s="70" t="s">
+      <c r="H24" s="69"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="67" t="s">
         <v>43</v>
       </c>
       <c r="K24" s="62" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="L24" s="64" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="M24" s="59"/>
       <c r="N24" s="59" t="s">

</xml_diff>